<commit_message>
more edits, need tons of editing
</commit_message>
<xml_diff>
--- a/Docs/LiPoBBSupply-BOM.xlsx
+++ b/Docs/LiPoBBSupply-BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17200" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20880" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>BOM #</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>LMT70</t>
-  </si>
-  <si>
     <t>Temperature Sensor Analog, Local -55°C ~ 150°C 5.194mV/°C 4-DSBGA (0.9x0.9)</t>
   </si>
   <si>
@@ -115,22 +112,49 @@
     <t>C1</t>
   </si>
   <si>
-    <t>0.10µF capacitor</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>LMT70 Breakout</t>
-  </si>
-  <si>
     <t>LMT70YFQT</t>
   </si>
   <si>
     <t>296-42088-1-ND</t>
   </si>
   <si>
-    <t>1/8 of 40 Pos Male Header Pins</t>
+    <t>JST Connector</t>
+  </si>
+  <si>
+    <t>LiPo</t>
+  </si>
+  <si>
+    <t>AP2210</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>1uF cap</t>
+  </si>
+  <si>
+    <t>2.2uF cap</t>
+  </si>
+  <si>
+    <t>1k resistor</t>
+  </si>
+  <si>
+    <t>LiPo Battery Breadboard Supply</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Shunt</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>100pF</t>
   </si>
 </sst>
 </file>
@@ -1400,7 +1424,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1421,7 +1445,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="26" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -1434,7 +1458,7 @@
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M1" s="18">
         <f>SUM(M3:M5)</f>
@@ -1487,31 +1511,31 @@
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>18</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>20</v>
-      </c>
       <c r="H3" s="11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K3" s="12">
         <v>1</v>
@@ -1529,31 +1553,31 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="F4" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="22" t="s">
+      <c r="H4" s="22" t="s">
         <v>23</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>24</v>
       </c>
       <c r="I4" s="22" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="13">
         <v>1</v>
@@ -1572,13 +1596,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>11</v>
@@ -1590,13 +1614,13 @@
         <v>15</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" s="22" t="s">
         <v>16</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="22">
         <v>1</v>
@@ -1610,22 +1634,50 @@
       </c>
     </row>
     <row r="6" spans="1:13">
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="M6" s="1"/>
     </row>
+    <row r="7" spans="1:13">
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="9" spans="1:13">
+      <c r="B9" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="I9" s="2"/>
       <c r="M9" s="6"/>
     </row>
     <row r="10" spans="1:13">
+      <c r="B10" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:13">
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:13">
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:13">
+      <c r="B13" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="I13" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to the silkscreen and changes to the BOM
</commit_message>
<xml_diff>
--- a/Docs/LiPoBBSupply-BOM.xlsx
+++ b/Docs/LiPoBBSupply-BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20880" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="81">
   <si>
     <t>BOM #</t>
   </si>
@@ -73,16 +73,64 @@
     <t>Digi-Key</t>
   </si>
   <si>
-    <t>Temperature Sensor Analog, Local -55°C ~ 150°C 5.194mV/°C 4-DSBGA (0.9x0.9)</t>
-  </si>
-  <si>
-    <t>4-DSBGA (0.9x0.9)</t>
-  </si>
-  <si>
-    <t>Texas Insruments</t>
-  </si>
-  <si>
-    <t>40 Positions Header, Breakaway Connector 0.100" (2.54mm) Through Hole Gold</t>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>JST Connector</t>
+  </si>
+  <si>
+    <t>LiPo</t>
+  </si>
+  <si>
+    <t>AP2210</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>2.2uF cap</t>
+  </si>
+  <si>
+    <t>1k resistor</t>
+  </si>
+  <si>
+    <t>LiPo Battery Breadboard Supply</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>Shunt</t>
+  </si>
+  <si>
+    <t>Linear Voltage Regulator IC Positive Fixed 1 Output 3.3V 300mA SOT-23-5</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
+  </si>
+  <si>
+    <t>Diodes Incorporated</t>
+  </si>
+  <si>
+    <t>AP2210K-3.3TRG1</t>
+  </si>
+  <si>
+    <t>AP2210K-3.3TRG1DICT-ND</t>
+  </si>
+  <si>
+    <t>JST Right Angle Connector - White</t>
+  </si>
+  <si>
+    <t>4UCOM Technology Inc.</t>
+  </si>
+  <si>
+    <t>Sparkfun Electronics</t>
+  </si>
+  <si>
+    <t>PRT-08612</t>
+  </si>
+  <si>
+    <t>LDO</t>
   </si>
   <si>
     <t>THT</t>
@@ -97,75 +145,136 @@
     <t>S1011EC-40-ND</t>
   </si>
   <si>
-    <t>JMP</t>
-  </si>
-  <si>
-    <t>0.10µF ±10% 16V Ceramic Capacitor X7R 0402 (1005 Metric)</t>
-  </si>
-  <si>
-    <t>CL05B104KO5NNNC</t>
-  </si>
-  <si>
-    <t>1276-1001-1-ND</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>LMT70YFQT</t>
-  </si>
-  <si>
-    <t>296-42088-1-ND</t>
-  </si>
-  <si>
-    <t>JST Connector</t>
-  </si>
-  <si>
-    <t>LiPo</t>
-  </si>
-  <si>
-    <t>AP2210</t>
-  </si>
-  <si>
-    <t>Headers</t>
-  </si>
-  <si>
-    <t>1uF cap</t>
-  </si>
-  <si>
-    <t>2.2uF cap</t>
-  </si>
-  <si>
-    <t>1k resistor</t>
-  </si>
-  <si>
-    <t>LiPo Battery Breadboard Supply</t>
-  </si>
-  <si>
-    <t>Switch</t>
-  </si>
-  <si>
-    <t>Shunt</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>100pF</t>
+    <t>12/40 Positions Header, Breakaway Connector 0.100" (2.54mm) Through Hole Gold</t>
+  </si>
+  <si>
+    <t>J2,J3</t>
+  </si>
+  <si>
+    <t>16V, X5R</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>GRM188R61C225KE15D</t>
+  </si>
+  <si>
+    <t>490-3296-1-ND</t>
+  </si>
+  <si>
+    <t>RES SMD 1.02K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>RC0402FR-071K02L</t>
+  </si>
+  <si>
+    <t>YAG3029CT-ND</t>
+  </si>
+  <si>
+    <t>47pF ±5% 50V Ceramic Capacitor C0G, NP0 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>CL05C470JB5NNNC</t>
+  </si>
+  <si>
+    <t>1276-1699-1-ND</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>47pF</t>
+  </si>
+  <si>
+    <t>SWITCH SLIDE DPDT 300MA 6V</t>
+  </si>
+  <si>
+    <t>J Lead</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>JS202011JCQN</t>
+  </si>
+  <si>
+    <t>CKN10723CT-ND</t>
+  </si>
+  <si>
+    <t>3V3.SWITCH</t>
+  </si>
+  <si>
+    <t>Green 571 nm, 2 V</t>
+  </si>
+  <si>
+    <t>Lite-On Inc</t>
+  </si>
+  <si>
+    <t>LTST-C190KGKT</t>
+  </si>
+  <si>
+    <t>160-1435-1-ND</t>
+  </si>
+  <si>
+    <t>3.3V,PWR</t>
+  </si>
+  <si>
+    <t>2 (1 x 2) Position Shunt Connector Black Open Top 0.100" (2.54mm) Gold</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>QPC02SXGN-RC</t>
+  </si>
+  <si>
+    <t>S9337-ND</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>C1,C2,C3,C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>100k resistor</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Green LED</t>
+  </si>
+  <si>
+    <t>R1,R2</t>
+  </si>
+  <si>
+    <t>100k Ohm ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Moisture Resistant Thick Film</t>
+  </si>
+  <si>
+    <t>RC0402FR-07100KL</t>
+  </si>
+  <si>
+    <t>311-100KLRCT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,6 +306,11 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
     </font>
@@ -245,7 +359,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="388">
+  <cellStyleXfs count="430">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -634,8 +748,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -673,9 +829,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -688,23 +841,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="388">
+  <cellStyles count="430">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -903,6 +1066,27 @@
     <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="401" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="419" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="421" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="423" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="425" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="427" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="429" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1092,6 +1276,27 @@
     <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="400" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="406" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="408" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="410" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="412" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="418" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="420" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="422" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="424" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="426" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="428" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1421,10 +1626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1439,33 +1644,80 @@
     <col min="8" max="8" width="18.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="3"/>
+    <col min="11" max="11" width="10.83203125" style="3"/>
+    <col min="12" max="12" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+    <row r="1" spans="1:35" ht="13">
+      <c r="A1" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
       <c r="E1" s="7"/>
       <c r="F1" s="8"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" s="18">
-        <f>SUM(M3:M5)</f>
-        <v>3.3824999999999998</v>
-      </c>
+      <c r="K1" s="23"/>
+      <c r="L1" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="17">
+        <f>SUM(M3:M15)</f>
+        <v>3.4820000000000002</v>
+      </c>
+      <c r="O1" s="29">
+        <f>SUM(O3:O12)</f>
+        <v>2.7942</v>
+      </c>
+      <c r="P1" s="29">
+        <f>SUM(P3:P15)</f>
+        <v>2.1797000000000004</v>
+      </c>
+      <c r="Q1" s="29">
+        <f>SUM(Q3:Q12)</f>
+        <v>2.1212599999999999</v>
+      </c>
+      <c r="R1" s="29">
+        <f>SUM(R3:R12)</f>
+        <v>1.8721000000000001</v>
+      </c>
+      <c r="S1" s="29">
+        <f>SUM(S3:S12)</f>
+        <v>1.7539899999999999</v>
+      </c>
+      <c r="U1" s="29">
+        <f>SUM(U3:U12)</f>
+        <v>69.855000000000004</v>
+      </c>
+      <c r="V1" s="29">
+        <f>SUM(V3:V12)</f>
+        <v>217.96999999999997</v>
+      </c>
+      <c r="W1" s="29">
+        <f>SUM(W3:W12)</f>
+        <v>530.31500000000005</v>
+      </c>
+      <c r="X1" s="29">
+        <f>SUM(X3:X12)</f>
+        <v>936.05000000000007</v>
+      </c>
+      <c r="Y1" s="29">
+        <f>SUM(Y3:Y12)</f>
+        <v>1753.99</v>
+      </c>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:35">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1497,188 +1749,872 @@
         <v>8</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>6</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="O2" s="30">
+        <v>25</v>
+      </c>
+      <c r="P2" s="30">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="30">
+        <v>250</v>
+      </c>
+      <c r="R2" s="30">
+        <v>500</v>
+      </c>
+      <c r="S2" s="30">
+        <v>1000</v>
+      </c>
+      <c r="T2" s="27"/>
+      <c r="U2" s="30">
+        <v>25</v>
+      </c>
+      <c r="V2" s="30">
+        <v>100</v>
+      </c>
+      <c r="W2" s="30">
+        <v>250</v>
+      </c>
+      <c r="X2" s="30">
+        <v>500</v>
+      </c>
+      <c r="Y2" s="30">
+        <v>1000</v>
+      </c>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="28"/>
+      <c r="AE2" s="28"/>
     </row>
-    <row r="3" spans="1:13" s="22" customFormat="1" ht="33">
+    <row r="3" spans="1:35" s="20" customFormat="1">
       <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>18</v>
+      <c r="F3" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>16</v>
+        <v>33</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="12">
+        <v>35</v>
+      </c>
+      <c r="K3" s="24">
+        <v>0.95</v>
+      </c>
+      <c r="L3" s="12">
         <v>1</v>
       </c>
-      <c r="L3" s="15">
-        <v>3.19</v>
-      </c>
-      <c r="M3" s="20">
-        <f>K3*L3</f>
-        <v>3.19</v>
-      </c>
+      <c r="M3" s="26">
+        <f>L3*K3</f>
+        <v>0.95</v>
+      </c>
+      <c r="O3" s="25">
+        <v>0.9</v>
+      </c>
+      <c r="P3" s="25">
+        <v>0.86</v>
+      </c>
+      <c r="Q3" s="25">
+        <v>0.86</v>
+      </c>
+      <c r="R3" s="25">
+        <v>0.86</v>
+      </c>
+      <c r="S3" s="25">
+        <v>0.86</v>
+      </c>
+      <c r="T3" s="25"/>
+      <c r="U3" s="6">
+        <f>O3*O$2</f>
+        <v>22.5</v>
+      </c>
+      <c r="V3" s="6">
+        <f>P3*P$2</f>
+        <v>86</v>
+      </c>
+      <c r="W3" s="6">
+        <f>Q3*Q$2</f>
+        <v>215</v>
+      </c>
+      <c r="X3" s="6">
+        <f>R3*R$2</f>
+        <v>430</v>
+      </c>
+      <c r="Y3" s="6">
+        <f>S3*S$2</f>
+        <v>860</v>
+      </c>
+      <c r="Z3" s="19"/>
+      <c r="AA3" s="19"/>
+      <c r="AB3" s="19"/>
+      <c r="AC3" s="19"/>
+      <c r="AD3" s="19"/>
+      <c r="AE3" s="19"/>
+      <c r="AF3" s="19"/>
+      <c r="AG3" s="19"/>
+      <c r="AH3" s="19"/>
+      <c r="AI3" s="19"/>
     </row>
-    <row r="4" spans="1:13" s="22" customFormat="1">
+    <row r="4" spans="1:35" s="20" customFormat="1">
       <c r="A4" s="11">
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="24">
+        <v>0.42</v>
+      </c>
+      <c r="L4" s="13">
+        <v>1</v>
+      </c>
+      <c r="M4" s="26">
+        <f t="shared" ref="M4:M15" si="0">L4*K4</f>
+        <v>0.42</v>
+      </c>
+      <c r="O4" s="25">
+        <v>0.317</v>
+      </c>
+      <c r="P4" s="25">
+        <v>0.1973</v>
+      </c>
+      <c r="Q4" s="25">
+        <v>0.1973</v>
+      </c>
+      <c r="R4" s="25">
+        <v>0.13496</v>
+      </c>
+      <c r="S4" s="25">
+        <v>0.10382</v>
+      </c>
+      <c r="T4" s="25"/>
+      <c r="U4" s="6">
+        <f t="shared" ref="U4:Y12" si="1">O4*O$2</f>
+        <v>7.9249999999999998</v>
+      </c>
+      <c r="V4" s="6">
+        <f t="shared" si="1"/>
+        <v>19.73</v>
+      </c>
+      <c r="W4" s="6">
+        <f t="shared" si="1"/>
+        <v>49.325000000000003</v>
+      </c>
+      <c r="X4" s="6">
+        <f t="shared" si="1"/>
+        <v>67.48</v>
+      </c>
+      <c r="Y4" s="6">
+        <f t="shared" si="1"/>
+        <v>103.82</v>
+      </c>
+      <c r="Z4" s="19"/>
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="19"/>
+      <c r="AE4" s="19"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
+      <c r="AH4" s="19"/>
+      <c r="AI4" s="19"/>
+    </row>
+    <row r="5" spans="1:35" s="20" customFormat="1">
+      <c r="A5" s="20">
+        <v>3</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="25">
+        <f>(12/40)*0.74</f>
+        <v>0.222</v>
+      </c>
+      <c r="L5" s="20">
+        <v>1</v>
+      </c>
+      <c r="M5" s="26">
+        <f t="shared" si="0"/>
+        <v>0.222</v>
+      </c>
+      <c r="O5" s="25">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="P5" s="25">
+        <v>0.54179999999999995</v>
+      </c>
+      <c r="Q5" s="25">
+        <v>0.54179999999999995</v>
+      </c>
+      <c r="R5" s="25">
+        <v>0.42827999999999999</v>
+      </c>
+      <c r="S5" s="25">
+        <v>0.36764999999999998</v>
+      </c>
+      <c r="T5" s="25"/>
+      <c r="U5" s="6">
+        <f t="shared" si="1"/>
+        <v>16.45</v>
+      </c>
+      <c r="V5" s="6">
+        <f t="shared" si="1"/>
+        <v>54.179999999999993</v>
+      </c>
+      <c r="W5" s="6">
+        <f t="shared" si="1"/>
+        <v>135.44999999999999</v>
+      </c>
+      <c r="X5" s="6">
+        <f t="shared" si="1"/>
+        <v>214.14</v>
+      </c>
+      <c r="Y5" s="6">
+        <f t="shared" si="1"/>
+        <v>367.65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="L6" s="3">
+        <v>2</v>
+      </c>
+      <c r="M6" s="26">
+        <f t="shared" si="0"/>
+        <v>0.24</v>
+      </c>
+      <c r="O6" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="P6" s="6">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>3.2320000000000002E-2</v>
+      </c>
+      <c r="R6" s="25">
+        <v>2.7060000000000001E-2</v>
+      </c>
+      <c r="S6" s="6">
+        <v>2.222E-2</v>
+      </c>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="V6" s="6">
+        <f t="shared" si="1"/>
+        <v>3.84</v>
+      </c>
+      <c r="W6" s="6">
+        <f t="shared" si="1"/>
+        <v>8.08</v>
+      </c>
+      <c r="X6" s="6">
+        <f t="shared" si="1"/>
+        <v>13.530000000000001</v>
+      </c>
+      <c r="Y6" s="6">
+        <f t="shared" si="1"/>
+        <v>22.22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2</v>
+      </c>
+      <c r="M7" s="26">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="O7" s="6">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="P7" s="6">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>3.6800000000000001E-3</v>
+      </c>
+      <c r="R7" s="25">
+        <v>2.96E-3</v>
+      </c>
+      <c r="S7" s="6">
+        <v>2.1700000000000001E-3</v>
+      </c>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
+      <c r="V7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.48</v>
+      </c>
+      <c r="W7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.92</v>
+      </c>
+      <c r="X7" s="6">
+        <f t="shared" si="1"/>
+        <v>1.48</v>
+      </c>
+      <c r="Y7" s="6">
+        <f t="shared" si="1"/>
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="L8" s="3">
+        <v>2</v>
+      </c>
+      <c r="M8" s="26">
+        <f t="shared" ref="M8" si="2">L8*K8</f>
+        <v>0.2</v>
+      </c>
+      <c r="O8" s="6">
+        <v>0.13</v>
+      </c>
+      <c r="P8" s="6">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="R8" s="25">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="S8" s="6">
+        <v>2.4199999999999998E-3</v>
+      </c>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6">
+        <f>O8*O$2</f>
+        <v>3.25</v>
+      </c>
+      <c r="V8" s="6">
+        <f t="shared" ref="V8" si="3">P8*P$2</f>
+        <v>0.54</v>
+      </c>
+      <c r="W8" s="6">
+        <f t="shared" ref="W8" si="4">Q8*Q$2</f>
+        <v>1.35</v>
+      </c>
+      <c r="X8" s="6">
+        <f t="shared" ref="X8" si="5">R8*R$2</f>
+        <v>2.7</v>
+      </c>
+      <c r="Y8" s="6">
+        <f t="shared" ref="Y8" si="6">S8*S$2</f>
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="22" t="s">
+      <c r="C9" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="13">
+      <c r="J9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.48</v>
+      </c>
+      <c r="L9" s="3">
         <v>1</v>
       </c>
-      <c r="L4" s="15">
-        <f>0.74/8</f>
-        <v>9.2499999999999999E-2</v>
-      </c>
-      <c r="M4" s="20">
-        <f t="shared" ref="M4:M5" si="0">K4*L4</f>
-        <v>9.2499999999999999E-2</v>
+      <c r="M9" s="26">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+      <c r="O9" s="6">
+        <v>0.45240000000000002</v>
+      </c>
+      <c r="P9" s="6">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0.37356</v>
+      </c>
+      <c r="R9" s="25">
+        <v>0.31762000000000001</v>
+      </c>
+      <c r="S9" s="25">
+        <v>0.31762000000000001</v>
+      </c>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6">
+        <f t="shared" si="1"/>
+        <v>11.31</v>
+      </c>
+      <c r="V9" s="6">
+        <f t="shared" si="1"/>
+        <v>38.5</v>
+      </c>
+      <c r="W9" s="6">
+        <f t="shared" si="1"/>
+        <v>93.39</v>
+      </c>
+      <c r="X9" s="6">
+        <f t="shared" si="1"/>
+        <v>158.81</v>
+      </c>
+      <c r="Y9" s="6">
+        <f t="shared" si="1"/>
+        <v>317.62</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="22" customFormat="1">
-      <c r="A5" s="22">
-        <v>3</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="23" t="s">
+    <row r="10" spans="1:35">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="C10" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" s="32">
+        <v>0.13</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="26">
+        <f t="shared" si="0"/>
+        <v>0.13</v>
+      </c>
+      <c r="O10" s="6">
+        <v>5.4800000000000001E-2</v>
+      </c>
+      <c r="P10" s="6">
+        <v>3.85E-2</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>3.2559999999999999E-2</v>
+      </c>
+      <c r="R10" s="25">
+        <v>3.0099999999999998E-2</v>
+      </c>
+      <c r="S10" s="6">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6">
+        <f t="shared" si="1"/>
+        <v>1.37</v>
+      </c>
+      <c r="V10" s="6">
+        <f t="shared" si="1"/>
+        <v>3.85</v>
+      </c>
+      <c r="W10" s="6">
+        <f t="shared" si="1"/>
+        <v>8.1399999999999988</v>
+      </c>
+      <c r="X10" s="6">
+        <f t="shared" si="1"/>
+        <v>15.049999999999999</v>
+      </c>
+      <c r="Y10" s="6">
+        <f t="shared" si="1"/>
+        <v>26.599999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="24" t="s">
+      <c r="F11" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" s="32">
+        <v>0.27</v>
+      </c>
+      <c r="L11" s="3">
+        <v>2</v>
+      </c>
+      <c r="M11" s="26">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
+      </c>
+      <c r="O11" s="6">
+        <v>0.14480000000000001</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0.10340000000000001</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>7.0319999999999994E-2</v>
+      </c>
+      <c r="R11" s="25">
+        <v>6.2039999999999998E-2</v>
+      </c>
+      <c r="S11" s="6">
+        <v>4.8599999999999997E-2</v>
+      </c>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6">
+        <f t="shared" si="1"/>
+        <v>3.62</v>
+      </c>
+      <c r="V11" s="6">
+        <f t="shared" si="1"/>
+        <v>10.34</v>
+      </c>
+      <c r="W11" s="6">
+        <f t="shared" si="1"/>
+        <v>17.579999999999998</v>
+      </c>
+      <c r="X11" s="6">
+        <f t="shared" si="1"/>
+        <v>31.02</v>
+      </c>
+      <c r="Y11" s="6">
+        <f t="shared" si="1"/>
+        <v>48.599999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="22" t="s">
+      <c r="H12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="22">
+      <c r="J12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="L12" s="3">
         <v>1</v>
       </c>
-      <c r="L5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="M5" s="20">
+      <c r="M12" s="26">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
+      <c r="O12" s="6">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="P12" s="6">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>4.3200000000000001E-3</v>
+      </c>
+      <c r="R12" s="25">
+        <v>3.6800000000000001E-3</v>
+      </c>
+      <c r="S12" s="6">
+        <v>2.8900000000000002E-3</v>
+      </c>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6">
+        <f t="shared" si="1"/>
+        <v>0.21</v>
+      </c>
+      <c r="V12" s="6">
+        <f t="shared" si="1"/>
+        <v>0.51</v>
+      </c>
+      <c r="W12" s="6">
+        <f t="shared" si="1"/>
+        <v>1.08</v>
+      </c>
+      <c r="X12" s="6">
+        <f t="shared" si="1"/>
+        <v>1.84</v>
+      </c>
+      <c r="Y12" s="6">
+        <f t="shared" si="1"/>
+        <v>2.89</v>
+      </c>
     </row>
-    <row r="6" spans="1:13">
-      <c r="B6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="1"/>
+    <row r="13" spans="1:35">
+      <c r="K13" s="6"/>
+      <c r="M13" s="26"/>
+      <c r="P13" s="26"/>
     </row>
-    <row r="7" spans="1:13">
-      <c r="B7" s="3" t="s">
-        <v>38</v>
-      </c>
+    <row r="14" spans="1:35">
+      <c r="K14" s="6"/>
+      <c r="M14" s="26"/>
+      <c r="P14" s="26"/>
     </row>
-    <row r="8" spans="1:13">
-      <c r="B8" s="3" t="s">
-        <v>39</v>
-      </c>
+    <row r="15" spans="1:35">
+      <c r="K15" s="6"/>
+      <c r="M15" s="26"/>
+      <c r="P15" s="26"/>
     </row>
-    <row r="9" spans="1:13">
-      <c r="B9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="M9" s="6"/>
+    <row r="16" spans="1:35">
+      <c r="M16" s="6"/>
+      <c r="P16" s="6"/>
     </row>
-    <row r="10" spans="1:13">
-      <c r="B10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="B11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="B12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="B13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="2"/>
+    <row r="17" spans="13:16">
+      <c r="M17" s="6"/>
+      <c r="P17" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
changes to BOM and change in value of Cbypass on regulator in schematic
</commit_message>
<xml_diff>
--- a/Docs/LiPoBBSupply-BOM.xlsx
+++ b/Docs/LiPoBBSupply-BOM.xlsx
@@ -791,7 +791,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -855,17 +855,19 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="8" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="430">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1629,7 +1631,7 @@
   <dimension ref="A1:AI17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -1646,16 +1648,18 @@
     <col min="10" max="10" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" style="3"/>
     <col min="12" max="12" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="3"/>
+    <col min="13" max="14" width="10.83203125" style="3"/>
+    <col min="15" max="26" width="10.83203125" style="32"/>
+    <col min="27" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="13">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="7"/>
       <c r="F1" s="8"/>
       <c r="G1" s="7"/>
@@ -1670,47 +1674,17 @@
         <f>SUM(M3:M15)</f>
         <v>3.4820000000000002</v>
       </c>
-      <c r="O1" s="29">
-        <f>SUM(O3:O12)</f>
-        <v>2.7942</v>
-      </c>
-      <c r="P1" s="29">
-        <f>SUM(P3:P15)</f>
-        <v>2.1797000000000004</v>
-      </c>
-      <c r="Q1" s="29">
-        <f>SUM(Q3:Q12)</f>
-        <v>2.1212599999999999</v>
-      </c>
-      <c r="R1" s="29">
-        <f>SUM(R3:R12)</f>
-        <v>1.8721000000000001</v>
-      </c>
-      <c r="S1" s="29">
-        <f>SUM(S3:S12)</f>
-        <v>1.7539899999999999</v>
-      </c>
-      <c r="U1" s="29">
-        <f>SUM(U3:U12)</f>
-        <v>69.855000000000004</v>
-      </c>
-      <c r="V1" s="29">
-        <f>SUM(V3:V12)</f>
-        <v>217.96999999999997</v>
-      </c>
-      <c r="W1" s="29">
-        <f>SUM(W3:W12)</f>
-        <v>530.31500000000005</v>
-      </c>
-      <c r="X1" s="29">
-        <f>SUM(X3:X12)</f>
-        <v>936.05000000000007</v>
-      </c>
-      <c r="Y1" s="29">
-        <f>SUM(Y3:Y12)</f>
-        <v>1753.99</v>
-      </c>
-      <c r="Z1" s="1"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="33"/>
       <c r="AA1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
@@ -1757,42 +1731,22 @@
       <c r="M2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="30">
-        <v>25</v>
-      </c>
-      <c r="P2" s="30">
-        <v>100</v>
-      </c>
-      <c r="Q2" s="30">
-        <v>250</v>
-      </c>
-      <c r="R2" s="30">
-        <v>500</v>
-      </c>
-      <c r="S2" s="30">
-        <v>1000</v>
-      </c>
-      <c r="T2" s="27"/>
-      <c r="U2" s="30">
-        <v>25</v>
-      </c>
-      <c r="V2" s="30">
-        <v>100</v>
-      </c>
-      <c r="W2" s="30">
-        <v>250</v>
-      </c>
-      <c r="X2" s="30">
-        <v>500</v>
-      </c>
-      <c r="Y2" s="30">
-        <v>1000</v>
-      </c>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="28"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
     </row>
     <row r="3" spans="1:35" s="20" customFormat="1">
       <c r="A3" s="11">
@@ -1833,43 +1787,18 @@
         <f>L3*K3</f>
         <v>0.95</v>
       </c>
-      <c r="O3" s="25">
-        <v>0.9</v>
-      </c>
-      <c r="P3" s="25">
-        <v>0.86</v>
-      </c>
-      <c r="Q3" s="25">
-        <v>0.86</v>
-      </c>
-      <c r="R3" s="25">
-        <v>0.86</v>
-      </c>
-      <c r="S3" s="25">
-        <v>0.86</v>
-      </c>
-      <c r="T3" s="25"/>
-      <c r="U3" s="6">
-        <f>O3*O$2</f>
-        <v>22.5</v>
-      </c>
-      <c r="V3" s="6">
-        <f>P3*P$2</f>
-        <v>86</v>
-      </c>
-      <c r="W3" s="6">
-        <f>Q3*Q$2</f>
-        <v>215</v>
-      </c>
-      <c r="X3" s="6">
-        <f>R3*R$2</f>
-        <v>430</v>
-      </c>
-      <c r="Y3" s="6">
-        <f>S3*S$2</f>
-        <v>860</v>
-      </c>
-      <c r="Z3" s="19"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="33"/>
       <c r="AA3" s="19"/>
       <c r="AB3" s="19"/>
       <c r="AC3" s="19"/>
@@ -1890,25 +1819,25 @@
       <c r="C4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="27" t="s">
         <v>31</v>
       </c>
       <c r="K4" s="24">
@@ -1918,46 +1847,21 @@
         <v>1</v>
       </c>
       <c r="M4" s="26">
-        <f t="shared" ref="M4:M15" si="0">L4*K4</f>
+        <f t="shared" ref="M4:M12" si="0">L4*K4</f>
         <v>0.42</v>
       </c>
-      <c r="O4" s="25">
-        <v>0.317</v>
-      </c>
-      <c r="P4" s="25">
-        <v>0.1973</v>
-      </c>
-      <c r="Q4" s="25">
-        <v>0.1973</v>
-      </c>
-      <c r="R4" s="25">
-        <v>0.13496</v>
-      </c>
-      <c r="S4" s="25">
-        <v>0.10382</v>
-      </c>
-      <c r="T4" s="25"/>
-      <c r="U4" s="6">
-        <f t="shared" ref="U4:Y12" si="1">O4*O$2</f>
-        <v>7.9249999999999998</v>
-      </c>
-      <c r="V4" s="6">
-        <f t="shared" si="1"/>
-        <v>19.73</v>
-      </c>
-      <c r="W4" s="6">
-        <f t="shared" si="1"/>
-        <v>49.325000000000003</v>
-      </c>
-      <c r="X4" s="6">
-        <f t="shared" si="1"/>
-        <v>67.48</v>
-      </c>
-      <c r="Y4" s="6">
-        <f t="shared" si="1"/>
-        <v>103.82</v>
-      </c>
-      <c r="Z4" s="19"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="31"/>
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="33"/>
       <c r="AA4" s="19"/>
       <c r="AB4" s="19"/>
       <c r="AC4" s="19"/>
@@ -2010,42 +1914,18 @@
         <f t="shared" si="0"/>
         <v>0.222</v>
       </c>
-      <c r="O5" s="25">
-        <v>0.65800000000000003</v>
-      </c>
-      <c r="P5" s="25">
-        <v>0.54179999999999995</v>
-      </c>
-      <c r="Q5" s="25">
-        <v>0.54179999999999995</v>
-      </c>
-      <c r="R5" s="25">
-        <v>0.42827999999999999</v>
-      </c>
-      <c r="S5" s="25">
-        <v>0.36764999999999998</v>
-      </c>
-      <c r="T5" s="25"/>
-      <c r="U5" s="6">
-        <f t="shared" si="1"/>
-        <v>16.45</v>
-      </c>
-      <c r="V5" s="6">
-        <f t="shared" si="1"/>
-        <v>54.179999999999993</v>
-      </c>
-      <c r="W5" s="6">
-        <f t="shared" si="1"/>
-        <v>135.44999999999999</v>
-      </c>
-      <c r="X5" s="6">
-        <f t="shared" si="1"/>
-        <v>214.14</v>
-      </c>
-      <c r="Y5" s="6">
-        <f t="shared" si="1"/>
-        <v>367.65</v>
-      </c>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
+      <c r="Z5" s="32"/>
     </row>
     <row r="6" spans="1:35">
       <c r="A6" s="3">
@@ -2088,42 +1968,17 @@
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
-      <c r="O6" s="6">
-        <v>0.12</v>
-      </c>
-      <c r="P6" s="6">
-        <v>3.8399999999999997E-2</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>3.2320000000000002E-2</v>
-      </c>
-      <c r="R6" s="25">
-        <v>2.7060000000000001E-2</v>
-      </c>
-      <c r="S6" s="6">
-        <v>2.222E-2</v>
-      </c>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="V6" s="6">
-        <f t="shared" si="1"/>
-        <v>3.84</v>
-      </c>
-      <c r="W6" s="6">
-        <f t="shared" si="1"/>
-        <v>8.08</v>
-      </c>
-      <c r="X6" s="6">
-        <f t="shared" si="1"/>
-        <v>13.530000000000001</v>
-      </c>
-      <c r="Y6" s="6">
-        <f t="shared" si="1"/>
-        <v>22.22</v>
-      </c>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="31"/>
     </row>
     <row r="7" spans="1:35">
       <c r="A7" s="3">
@@ -2135,19 +1990,19 @@
       <c r="C7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="28" t="s">
+      <c r="H7" s="27" t="s">
         <v>49</v>
       </c>
       <c r="I7" s="3" t="s">
@@ -2166,42 +2021,17 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="O7" s="6">
-        <v>8.8000000000000005E-3</v>
-      </c>
-      <c r="P7" s="6">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>3.6800000000000001E-3</v>
-      </c>
-      <c r="R7" s="25">
-        <v>2.96E-3</v>
-      </c>
-      <c r="S7" s="6">
-        <v>2.1700000000000001E-3</v>
-      </c>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6">
-        <f t="shared" si="1"/>
-        <v>0.22</v>
-      </c>
-      <c r="V7" s="6">
-        <f t="shared" si="1"/>
-        <v>0.48</v>
-      </c>
-      <c r="W7" s="6">
-        <f t="shared" si="1"/>
-        <v>0.92</v>
-      </c>
-      <c r="X7" s="6">
-        <f t="shared" si="1"/>
-        <v>1.48</v>
-      </c>
-      <c r="Y7" s="6">
-        <f t="shared" si="1"/>
-        <v>2.17</v>
-      </c>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="31"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="31"/>
+      <c r="Y7" s="31"/>
     </row>
     <row r="8" spans="1:35">
       <c r="A8" s="3">
@@ -2213,19 +2043,19 @@
       <c r="C8" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="28" t="s">
         <v>79</v>
       </c>
       <c r="I8" s="3" t="s">
@@ -2241,45 +2071,20 @@
         <v>2</v>
       </c>
       <c r="M8" s="26">
-        <f t="shared" ref="M8" si="2">L8*K8</f>
+        <f t="shared" ref="M8" si="1">L8*K8</f>
         <v>0.2</v>
       </c>
-      <c r="O8" s="6">
-        <v>0.13</v>
-      </c>
-      <c r="P8" s="6">
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="Q8" s="6">
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="R8" s="25">
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="S8" s="6">
-        <v>2.4199999999999998E-3</v>
-      </c>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6">
-        <f>O8*O$2</f>
-        <v>3.25</v>
-      </c>
-      <c r="V8" s="6">
-        <f t="shared" ref="V8" si="3">P8*P$2</f>
-        <v>0.54</v>
-      </c>
-      <c r="W8" s="6">
-        <f t="shared" ref="W8" si="4">Q8*Q$2</f>
-        <v>1.35</v>
-      </c>
-      <c r="X8" s="6">
-        <f t="shared" ref="X8" si="5">R8*R$2</f>
-        <v>2.7</v>
-      </c>
-      <c r="Y8" s="6">
-        <f t="shared" ref="Y8" si="6">S8*S$2</f>
-        <v>2.42</v>
-      </c>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
     </row>
     <row r="9" spans="1:35">
       <c r="A9" s="3">
@@ -2322,42 +2127,17 @@
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
-      <c r="O9" s="6">
-        <v>0.45240000000000002</v>
-      </c>
-      <c r="P9" s="6">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="Q9" s="6">
-        <v>0.37356</v>
-      </c>
-      <c r="R9" s="25">
-        <v>0.31762000000000001</v>
-      </c>
-      <c r="S9" s="25">
-        <v>0.31762000000000001</v>
-      </c>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6">
-        <f t="shared" si="1"/>
-        <v>11.31</v>
-      </c>
-      <c r="V9" s="6">
-        <f t="shared" si="1"/>
-        <v>38.5</v>
-      </c>
-      <c r="W9" s="6">
-        <f t="shared" si="1"/>
-        <v>93.39</v>
-      </c>
-      <c r="X9" s="6">
-        <f t="shared" si="1"/>
-        <v>158.81</v>
-      </c>
-      <c r="Y9" s="6">
-        <f t="shared" si="1"/>
-        <v>317.62</v>
-      </c>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="31"/>
     </row>
     <row r="10" spans="1:35">
       <c r="A10" s="3">
@@ -2390,7 +2170,7 @@
       <c r="J10" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="32">
+      <c r="K10" s="29">
         <v>0.13</v>
       </c>
       <c r="L10" s="3">
@@ -2400,42 +2180,17 @@
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
-      <c r="O10" s="6">
-        <v>5.4800000000000001E-2</v>
-      </c>
-      <c r="P10" s="6">
-        <v>3.85E-2</v>
-      </c>
-      <c r="Q10" s="6">
-        <v>3.2559999999999999E-2</v>
-      </c>
-      <c r="R10" s="25">
-        <v>3.0099999999999998E-2</v>
-      </c>
-      <c r="S10" s="6">
-        <v>2.6599999999999999E-2</v>
-      </c>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6">
-        <f t="shared" si="1"/>
-        <v>1.37</v>
-      </c>
-      <c r="V10" s="6">
-        <f t="shared" si="1"/>
-        <v>3.85</v>
-      </c>
-      <c r="W10" s="6">
-        <f t="shared" si="1"/>
-        <v>8.1399999999999988</v>
-      </c>
-      <c r="X10" s="6">
-        <f t="shared" si="1"/>
-        <v>15.049999999999999</v>
-      </c>
-      <c r="Y10" s="6">
-        <f t="shared" si="1"/>
-        <v>26.599999999999998</v>
-      </c>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="31"/>
     </row>
     <row r="11" spans="1:35">
       <c r="A11" s="3">
@@ -2468,7 +2223,7 @@
       <c r="J11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K11" s="32">
+      <c r="K11" s="29">
         <v>0.27</v>
       </c>
       <c r="L11" s="3">
@@ -2478,42 +2233,17 @@
         <f t="shared" si="0"/>
         <v>0.54</v>
       </c>
-      <c r="O11" s="6">
-        <v>0.14480000000000001</v>
-      </c>
-      <c r="P11" s="6">
-        <v>0.10340000000000001</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>7.0319999999999994E-2</v>
-      </c>
-      <c r="R11" s="25">
-        <v>6.2039999999999998E-2</v>
-      </c>
-      <c r="S11" s="6">
-        <v>4.8599999999999997E-2</v>
-      </c>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6">
-        <f t="shared" si="1"/>
-        <v>3.62</v>
-      </c>
-      <c r="V11" s="6">
-        <f t="shared" si="1"/>
-        <v>10.34</v>
-      </c>
-      <c r="W11" s="6">
-        <f t="shared" si="1"/>
-        <v>17.579999999999998</v>
-      </c>
-      <c r="X11" s="6">
-        <f t="shared" si="1"/>
-        <v>31.02</v>
-      </c>
-      <c r="Y11" s="6">
-        <f t="shared" si="1"/>
-        <v>48.599999999999994</v>
-      </c>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="31"/>
     </row>
     <row r="12" spans="1:35">
       <c r="A12" s="3">
@@ -2556,65 +2286,40 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="O12" s="6">
-        <v>8.3999999999999995E-3</v>
-      </c>
-      <c r="P12" s="6">
-        <v>5.1000000000000004E-3</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>4.3200000000000001E-3</v>
-      </c>
-      <c r="R12" s="25">
-        <v>3.6800000000000001E-3</v>
-      </c>
-      <c r="S12" s="6">
-        <v>2.8900000000000002E-3</v>
-      </c>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6">
-        <f t="shared" si="1"/>
-        <v>0.21</v>
-      </c>
-      <c r="V12" s="6">
-        <f t="shared" si="1"/>
-        <v>0.51</v>
-      </c>
-      <c r="W12" s="6">
-        <f t="shared" si="1"/>
-        <v>1.08</v>
-      </c>
-      <c r="X12" s="6">
-        <f t="shared" si="1"/>
-        <v>1.84</v>
-      </c>
-      <c r="Y12" s="6">
-        <f t="shared" si="1"/>
-        <v>2.89</v>
-      </c>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="31"/>
+      <c r="Y12" s="31"/>
     </row>
     <row r="13" spans="1:35">
       <c r="K13" s="6"/>
       <c r="M13" s="26"/>
-      <c r="P13" s="26"/>
+      <c r="P13" s="24"/>
     </row>
     <row r="14" spans="1:35">
       <c r="K14" s="6"/>
       <c r="M14" s="26"/>
-      <c r="P14" s="26"/>
+      <c r="P14" s="24"/>
     </row>
     <row r="15" spans="1:35">
       <c r="K15" s="6"/>
       <c r="M15" s="26"/>
-      <c r="P15" s="26"/>
+      <c r="P15" s="24"/>
     </row>
     <row r="16" spans="1:35">
       <c r="M16" s="6"/>
-      <c r="P16" s="6"/>
+      <c r="P16" s="31"/>
     </row>
     <row r="17" spans="13:16">
       <c r="M17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="P17" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>